<commit_message>
bug fix on employee in bulk
</commit_message>
<xml_diff>
--- a/src/public/employeetemplate2.xlsx
+++ b/src/public/employeetemplate2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\__scorpion_\Desktop\New folder\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F3FFD48E-A5D4-4E29-92C7-1636E2BD72F9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1DCA688-8D3F-4A1B-89E3-3F062EFB0C1D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8940" xr2:uid="{0F0D9703-A8B6-4853-94FD-6DD23239D8D1}"/>
   </bookViews>
@@ -54,15 +54,6 @@
     <t>role</t>
   </si>
   <si>
-    <t>test1</t>
-  </si>
-  <si>
-    <t>test2</t>
-  </si>
-  <si>
-    <t>test4@gmail.com</t>
-  </si>
-  <si>
     <t>Kenya</t>
   </si>
   <si>
@@ -76,6 +67,15 @@
   </si>
   <si>
     <t>0769347882</t>
+  </si>
+  <si>
+    <t>leon</t>
+  </si>
+  <si>
+    <t>kibdne</t>
+  </si>
+  <si>
+    <t>kinde@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -470,7 +470,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -517,31 +517,31 @@
     </row>
     <row r="2" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" t="s">
+      <c r="E2" t="s">
         <v>10</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" t="s">
-        <v>13</v>
       </c>
       <c r="F2">
         <v>100</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="I2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>